<commit_message>
Revert "Merge branch 'master' of https://github.com/MissouriMRDT/TM4C129-Breakout_Hardware"
This reverts commit e6cd920ed13198a4f7d11fd6171e0ba52050bff9, reversing
changes made to e15dd7d36717f2d892901729c8f3941fb424f385.
</commit_message>
<xml_diff>
--- a/Documentation/TM4C129-Breakout_Hardware_2020-R1_BOM.xlsx
+++ b/Documentation/TM4C129-Breakout_Hardware_2020-R1_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\Rover\GitHub\Hardware\TM4C129-Breakout_Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F003501F-E4E8-4DB2-8D0E-578E83866307}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6254B1E-5B38-4D89-B44E-3AA7ECD90BF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -424,9 +424,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/pulse-electronics-network/HX1198FNLT/553-2209-1-ND/4168378</t>
-  </si>
-  <si>
-    <t>1uF</t>
   </si>
 </sst>
 </file>
@@ -817,10 +814,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1433,14 +1430,14 @@
         <v>63</v>
       </c>
       <c r="K17" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L17">
         <v>0.1</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="O17" s="6" t="s">
         <v>94</v>
@@ -1697,26 +1694,6 @@
       <c r="O24" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>25</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="J25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1</v>
-      </c>
-      <c r="O25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/MissouriMRDT/TM4C129-Breakout_Hardware""
This reverts commit 4686fe645caf3e9fbf8c00f0c0ea95986b0ea6b8.
</commit_message>
<xml_diff>
--- a/Documentation/TM4C129-Breakout_Hardware_2020-R1_BOM.xlsx
+++ b/Documentation/TM4C129-Breakout_Hardware_2020-R1_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\Rover\GitHub\Hardware\TM4C129-Breakout_Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6254B1E-5B38-4D89-B44E-3AA7ECD90BF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F003501F-E4E8-4DB2-8D0E-578E83866307}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
   <si>
     <t>Id</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/pulse-electronics-network/HX1198FNLT/553-2209-1-ND/4168378</t>
+  </si>
+  <si>
+    <t>1uF</t>
   </si>
 </sst>
 </file>
@@ -814,10 +817,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N24"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1430,14 +1433,14 @@
         <v>63</v>
       </c>
       <c r="K17" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L17">
         <v>0.1</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O17" s="6" t="s">
         <v>94</v>
@@ -1694,6 +1697,26 @@
       <c r="O24" s="6" t="s">
         <v>110</v>
       </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="J25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="O25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>